<commit_message>
Edit in CRC Cards #15 #18
</commit_message>
<xml_diff>
--- a/Structural Modeling/Question CRC.xlsx
+++ b/Structural Modeling/Question CRC.xlsx
@@ -18,13 +18,94 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+  <si>
+    <t>type: generic</t>
+  </si>
+  <si>
+    <t>associated use cases : 1</t>
+  </si>
+  <si>
+    <t>operations:</t>
+  </si>
+  <si>
+    <t>collaborators:</t>
+  </si>
+  <si>
+    <t>////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////</t>
+  </si>
+  <si>
+    <t>back</t>
+  </si>
+  <si>
+    <t>attributes</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>relationships</t>
+  </si>
+  <si>
+    <t>with</t>
+  </si>
+  <si>
+    <t>class name: question</t>
+  </si>
+  <si>
+    <t>Id: 5</t>
+  </si>
+  <si>
+    <t>answer</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>association</t>
+  </si>
+  <si>
+    <t>sprint</t>
+  </si>
+  <si>
+    <t>create question</t>
+  </si>
+  <si>
+    <t>user/sprint</t>
+  </si>
+  <si>
+    <t>answers</t>
+  </si>
+  <si>
+    <t>list&lt;(user,text)&gt;</t>
+  </si>
+  <si>
+    <t>report answers</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -49,8 +130,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -331,12 +418,155 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:B6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="53.5" customWidth="1"/>
+    <col min="2" max="2" width="30.625" customWidth="1"/>
+    <col min="3" max="3" width="22.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:3" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:3" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:3" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:3" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:2" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>